<commit_message>
Update designs + gerbers
</commit_message>
<xml_diff>
--- a/hardware/tools/diffprobe/diffprobe_eagle/bom_diffprobesimple.xlsx
+++ b/hardware/tools/diffprobe/diffprobe_eagle/bom_diffprobesimple.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="66">
   <si>
     <t>Line No.</t>
   </si>
@@ -205,6 +205,15 @@
   </si>
   <si>
     <t>SMA Female</t>
+  </si>
+  <si>
+    <t>2k</t>
+  </si>
+  <si>
+    <t>221R</t>
+  </si>
+  <si>
+    <t>10K</t>
   </si>
 </sst>
 </file>
@@ -562,7 +571,7 @@
   <dimension ref="A3:J19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="A3" sqref="A3:I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -725,6 +734,9 @@
       <c r="C8" s="2" t="s">
         <v>18</v>
       </c>
+      <c r="D8" s="2" t="s">
+        <v>63</v>
+      </c>
       <c r="H8" s="3" t="s">
         <v>12</v>
       </c>
@@ -739,6 +751,9 @@
       <c r="C9" s="2" t="s">
         <v>41</v>
       </c>
+      <c r="D9" s="2" t="s">
+        <v>64</v>
+      </c>
       <c r="H9" s="3" t="s">
         <v>12</v>
       </c>
@@ -784,6 +799,9 @@
       </c>
       <c r="C11" s="2" t="s">
         <v>43</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>65</v>
       </c>
       <c r="H11" s="3" t="s">
         <v>12</v>

</xml_diff>

<commit_message>
Update differential probe stuff
</commit_message>
<xml_diff>
--- a/hardware/tools/diffprobe/diffprobe_eagle/bom_diffprobesimple.xlsx
+++ b/hardware/tools/diffprobe/diffprobe_eagle/bom_diffprobesimple.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="99">
   <si>
     <t>Line No.</t>
   </si>
@@ -90,9 +90,6 @@
     <t>641-1014-1-ND</t>
   </si>
   <si>
-    <t xml:space="preserve"> CDBA120-G</t>
-  </si>
-  <si>
     <t>Comchip</t>
   </si>
   <si>
@@ -105,9 +102,6 @@
     <t>LNA</t>
   </si>
   <si>
-    <t>Total:</t>
-  </si>
-  <si>
     <t>AD8129ARZ</t>
   </si>
   <si>
@@ -207,13 +201,118 @@
     <t>SMA Female</t>
   </si>
   <si>
-    <t>2k</t>
-  </si>
-  <si>
-    <t>221R</t>
-  </si>
-  <si>
-    <t>10K</t>
+    <t>R11,R14</t>
+  </si>
+  <si>
+    <t>10k</t>
+  </si>
+  <si>
+    <t>0402</t>
+  </si>
+  <si>
+    <t>510R</t>
+  </si>
+  <si>
+    <t>R13</t>
+  </si>
+  <si>
+    <t>R15</t>
+  </si>
+  <si>
+    <t>25k</t>
+  </si>
+  <si>
+    <t>R16,R17</t>
+  </si>
+  <si>
+    <t>R12</t>
+  </si>
+  <si>
+    <t>4k7</t>
+  </si>
+  <si>
+    <t>C12, C13</t>
+  </si>
+  <si>
+    <t>C11</t>
+  </si>
+  <si>
+    <t>680pF</t>
+  </si>
+  <si>
+    <t>LM2903PWR</t>
+  </si>
+  <si>
+    <t>Texas Instruments</t>
+  </si>
+  <si>
+    <t>U2</t>
+  </si>
+  <si>
+    <t>LED1, LED2</t>
+  </si>
+  <si>
+    <t>LED3</t>
+  </si>
+  <si>
+    <t>Green LED</t>
+  </si>
+  <si>
+    <t>Red LED</t>
+  </si>
+  <si>
+    <t>296-6602-1-ND</t>
+  </si>
+  <si>
+    <t>Newark</t>
+  </si>
+  <si>
+    <t>LTST-C194KGKT</t>
+  </si>
+  <si>
+    <t>R5</t>
+  </si>
+  <si>
+    <t>R6,R7,R8,R9</t>
+  </si>
+  <si>
+    <t>Not Mounted</t>
+  </si>
+  <si>
+    <t>R10</t>
+  </si>
+  <si>
+    <t>1k, 1%</t>
+  </si>
+  <si>
+    <t>2k, 1%</t>
+  </si>
+  <si>
+    <t>221R, 1%</t>
+  </si>
+  <si>
+    <t>10K, 1%</t>
+  </si>
+  <si>
+    <t>49.9, 1%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MBR0540TPMSCT-ND </t>
+  </si>
+  <si>
+    <t>MBR0540-TP</t>
+  </si>
+  <si>
+    <t>CDBA120-G</t>
+  </si>
+  <si>
+    <t>Mouser</t>
+  </si>
+  <si>
+    <t>73251-1150</t>
+  </si>
+  <si>
+    <t>32M0773</t>
   </si>
 </sst>
 </file>
@@ -258,7 +357,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -267,6 +366,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -568,10 +671,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:J19"/>
+  <dimension ref="A3:K48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:I17"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -582,10 +685,12 @@
     <col min="6" max="6" width="20.42578125" customWidth="1"/>
     <col min="7" max="7" width="16.42578125" customWidth="1"/>
     <col min="8" max="8" width="16.28515625" customWidth="1"/>
-    <col min="9" max="9" width="18.28515625" customWidth="1"/>
+    <col min="9" max="9" width="28.28515625" customWidth="1"/>
+    <col min="10" max="10" width="13.28515625" customWidth="1"/>
+    <col min="11" max="11" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -616,8 +721,11 @@
       <c r="J3" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="K3" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>1</v>
       </c>
@@ -628,25 +736,25 @@
         <v>10</v>
       </c>
       <c r="E4" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F4" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="G4" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H4" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="I4" t="s">
         <v>31</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="I4" t="s">
-        <v>33</v>
       </c>
       <c r="J4" s="2">
         <v>4.51</v>
       </c>
     </row>
-    <row r="5" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>2</v>
       </c>
@@ -654,13 +762,13 @@
         <v>1</v>
       </c>
       <c r="C5" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F5" s="2" t="s">
         <v>34</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>36</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>17</v>
@@ -669,7 +777,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>3</v>
       </c>
@@ -677,7 +785,7 @@
         <v>4</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>11</v>
@@ -701,7 +809,7 @@
         <v>2.8000000000000001E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>4</v>
       </c>
@@ -709,13 +817,13 @@
         <v>1</v>
       </c>
       <c r="C7" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F7" s="2" t="s">
         <v>38</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>40</v>
       </c>
       <c r="G7" s="2" t="s">
         <v>17</v>
@@ -724,7 +832,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>5</v>
       </c>
@@ -732,33 +840,37 @@
         <v>1</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>18</v>
+        <v>72</v>
       </c>
       <c r="D8" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="F8"/>
+      <c r="G8"/>
+      <c r="H8" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="H8" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>6</v>
       </c>
       <c r="B9" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>41</v>
+        <v>71</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>64</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="F9"/>
+      <c r="G9"/>
       <c r="H9" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>7</v>
       </c>
@@ -766,31 +878,16 @@
         <v>1</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>42</v>
+        <v>18</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="H10" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="I10" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="J10" s="2">
-        <v>3.4</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
+        <v>89</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>8</v>
       </c>
@@ -798,152 +895,445 @@
         <v>1</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>65</v>
+        <v>90</v>
       </c>
       <c r="H11" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="2">
-        <v>9</v>
-      </c>
+    <row r="12" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B12" s="2">
         <v>1</v>
       </c>
       <c r="C12" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="J12" s="2">
+        <v>3.4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="2">
+        <v>1</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="2"/>
+      <c r="B14" s="2">
+        <v>1</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I14" s="2"/>
+      <c r="J14" s="2"/>
+    </row>
+    <row r="15" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="2">
+        <v>4</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="2">
+        <v>1</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="E16"/>
+      <c r="F16"/>
+      <c r="G16"/>
+      <c r="H16" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I16"/>
+      <c r="J16"/>
+    </row>
+    <row r="17" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="2">
+        <v>2</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="E17" s="4">
+        <v>0.01</v>
+      </c>
+      <c r="H17" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="2">
+        <v>1</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="E18" s="4">
+        <v>0.01</v>
+      </c>
+      <c r="H18" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="2">
+        <v>1</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="E19" s="4">
+        <v>0.01</v>
+      </c>
+      <c r="F19" s="3"/>
+      <c r="H19" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" s="2"/>
+      <c r="B20" s="2">
+        <v>1</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="E20" s="4">
+        <v>0.01</v>
+      </c>
+      <c r="H20" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="I20" s="2"/>
+      <c r="J20" s="2"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" s="2"/>
+      <c r="B21" s="2">
+        <v>2</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="E21" s="2"/>
+      <c r="H21" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="I21" s="2"/>
+      <c r="J21" s="2"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" s="2"/>
+      <c r="B22" s="2">
+        <v>1</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+      <c r="G22" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="I22" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="J22" s="2">
+        <v>0.63</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" s="2"/>
+      <c r="B23" s="2">
+        <v>1</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="F23" s="2"/>
+      <c r="G23" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="H23" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="I23" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="J23" s="2">
+        <v>0.82</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" s="2"/>
+      <c r="B24" s="2">
+        <v>1</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F24" t="s">
+        <v>94</v>
+      </c>
+      <c r="H24" t="s">
+        <v>45</v>
+      </c>
+      <c r="I24" t="s">
+        <v>93</v>
+      </c>
+      <c r="J24">
+        <v>0.47</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25" s="2"/>
+      <c r="B25" s="2">
+        <v>1</v>
+      </c>
+      <c r="C25" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="G12" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="H12" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="I12" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="J12" s="2">
-        <v>0.63</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="2">
-        <v>10</v>
-      </c>
-      <c r="B13" s="2">
-        <v>1</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="G13" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="H13" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="I13" s="2" t="s">
+      <c r="D25" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H25" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="I25" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="J25" s="2">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A26" s="2"/>
+      <c r="B26" s="2">
+        <v>2</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D26" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="J13" s="2">
-        <v>0.82</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="2">
-        <v>11</v>
-      </c>
-      <c r="B14" s="2">
-        <v>1</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E14" t="s">
-        <v>27</v>
-      </c>
-      <c r="H14" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="2">
+      <c r="E26" s="2"/>
+      <c r="F26" t="s">
+        <v>97</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="H26" s="2"/>
+      <c r="I26" s="2"/>
+      <c r="J26" s="2"/>
+      <c r="K26" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A27" s="2"/>
+      <c r="B27" s="2">
+        <v>1</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E27" s="2"/>
+      <c r="F27" s="2"/>
+      <c r="G27" s="2"/>
+      <c r="H27" s="2"/>
+      <c r="I27" s="2"/>
+      <c r="J27" s="2"/>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I28" s="2"/>
+      <c r="J28" s="2"/>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B29" s="2"/>
+      <c r="E29" s="2"/>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B30" s="2"/>
+      <c r="E30" s="2"/>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B31" s="2"/>
+      <c r="E31" s="2"/>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B32" s="2"/>
+      <c r="E32" s="2"/>
+    </row>
+    <row r="33" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K33" s="2"/>
+    </row>
+    <row r="34" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K34" s="2"/>
+    </row>
+    <row r="36" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K36" s="2"/>
+    </row>
+    <row r="37" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K37" s="2"/>
+    </row>
+    <row r="38" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K38" s="2"/>
+    </row>
+    <row r="39" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K39" s="2"/>
+    </row>
+    <row r="40" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="I40" s="2"/>
+      <c r="J40" s="2"/>
+      <c r="K40" s="2"/>
+    </row>
+    <row r="43" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B43" s="2"/>
+      <c r="C43" s="2"/>
+      <c r="D43" s="2"/>
+      <c r="E43" s="4"/>
+      <c r="H43" s="3"/>
+    </row>
+    <row r="46" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B46" s="2">
+        <v>2</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="E46" s="2"/>
+      <c r="F46" t="s">
+        <v>83</v>
+      </c>
+      <c r="H46" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B15" s="2">
-        <v>1</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="G15" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="H15" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="I15" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="J15" s="2">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="2">
-        <v>13</v>
-      </c>
-      <c r="B16" s="2">
-        <v>2</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="2">
-        <v>14</v>
-      </c>
-      <c r="B17" s="2">
-        <v>1</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="J17" s="2">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="19" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="I19" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="J19" s="2">
-        <f>SUM(J4:J18)</f>
-        <v>15.688000000000001</v>
+    </row>
+    <row r="47" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B47" s="2">
+        <v>1</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="E47" s="2"/>
+      <c r="H47" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="48" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B48" s="2">
+        <v>1</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="D48" s="2"/>
+      <c r="E48" s="2"/>
+      <c r="F48" t="s">
+        <v>74</v>
+      </c>
+      <c r="G48" t="s">
+        <v>75</v>
+      </c>
+      <c r="I48" t="s">
+        <v>81</v>
+      </c>
+      <c r="J48">
+        <v>0.51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>